<commit_message>
Clean Code - 1
</commit_message>
<xml_diff>
--- a/Upload/Example_Input.xlsx
+++ b/Upload/Example_Input.xlsx
@@ -1,12 +1,12 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="3280" yWindow="5600" windowWidth="25440" windowHeight="15000" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1" iterateDelta="0.0001"/>
@@ -438,7 +438,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
@@ -681,9 +681,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E3" r:id="rId1"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E4" r:id="rId2"/>
-    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="E5" r:id="rId3"/>
+    <hyperlink ref="E3" r:id="rId1"/>
+    <hyperlink ref="E4" r:id="rId2"/>
+    <hyperlink ref="E5" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>